<commit_message>
Update from Google Sheets
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -223,7 +223,7 @@
 Trading of electricity;
 Insurances;
 Purchase of consultancies;
-Responsability for the facilities;
+Responsibility for the facilities;
 O&amp;M strategy</t>
   </si>
   <si>
@@ -275,7 +275,7 @@
     <t>Rückabwicklung</t>
   </si>
   <si>
-    <t>wpl:8Decomissioning</t>
+    <t>wpl:8Decommissioning</t>
   </si>
   <si>
     <t>Planning of dismantling</t>

</xml_diff>